<commit_message>
fixed Employee login and search
</commit_message>
<xml_diff>
--- a/T4Dir/Data_Store.xlsx
+++ b/T4Dir/Data_Store.xlsx
@@ -1871,9 +1871,9 @@
           <t>T corp</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>a@gmail.com</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>asdfhuifwae</t>
         </is>
       </c>
     </row>

</xml_diff>